<commit_message>
exercice expression des besoins
</commit_message>
<xml_diff>
--- a/persistance_des_données/exercice_creation_cahier_des_charges/test_donnees_wagons.xlsx
+++ b/persistance_des_données/exercice_creation_cahier_des_charges/test_donnees_wagons.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
   <si>
     <t>données</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>numAtelier</t>
+  </si>
+  <si>
+    <t>nesle</t>
   </si>
 </sst>
 </file>
@@ -192,14 +195,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -216,13 +216,19 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -508,7 +514,7 @@
   <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,159 +525,159 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="4">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="A4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="4">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="7">
         <v>27905</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="3"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="4">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="B8" s="10"/>
+      <c r="C8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="4">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="3"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="4">
-        <v>1</v>
-      </c>
-      <c r="D11" s="3"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="6" t="s">
+      <c r="B12" s="10"/>
+      <c r="C12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
       <c r="C13" s="1">
         <v>1</v>
       </c>
@@ -680,23 +686,23 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="6" t="s">
+      <c r="B14" s="10"/>
+      <c r="C14" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="1">
         <v>1</v>
       </c>
@@ -708,20 +714,20 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="6" t="s">
+      <c r="B16" s="10"/>
+      <c r="C16" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
       <c r="C17" s="1">
         <v>1</v>
       </c>
@@ -730,20 +736,20 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="6" t="s">
+      <c r="B18" s="10"/>
+      <c r="C18" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
       <c r="C19" s="1">
         <v>1</v>
       </c>
@@ -752,55 +758,55 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="6" t="s">
+      <c r="B20" s="10"/>
+      <c r="C20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
       <c r="C21" s="1">
         <v>1</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="8">
         <v>44109</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="8">
         <v>44113</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="6" t="s">
+      <c r="B22" s="10"/>
+      <c r="C22" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
       <c r="C23" s="1">
         <v>1</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="9" t="s">
         <v>35</v>
       </c>
       <c r="E23" s="1">
@@ -808,48 +814,48 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="6" t="s">
+      <c r="B24" s="10"/>
+      <c r="C24" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
       <c r="C25" s="1">
         <v>1</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="8">
         <v>44108</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E25" s="8">
         <v>44115</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="6" t="s">
+      <c r="B26" s="10"/>
+      <c r="C26" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
       <c r="C27" s="1">
         <v>1</v>
       </c>
@@ -858,42 +864,42 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" s="6" t="s">
+      <c r="B28" s="10"/>
+      <c r="C28" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
       <c r="C29" s="1">
         <v>1</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" s="6" t="s">
+      <c r="B30" s="10"/>
+      <c r="C30" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
       <c r="C31" s="1">
         <v>1</v>
       </c>
@@ -902,28 +908,46 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="7"/>
-      <c r="C32" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
-      <c r="B34" s="9"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="9"/>
-      <c r="B35" s="9"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A10:B11"/>
+    <mergeCell ref="A12:B13"/>
+    <mergeCell ref="A14:B15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="A4:B5"/>
+    <mergeCell ref="A6:B7"/>
+    <mergeCell ref="A8:B9"/>
     <mergeCell ref="A28:B29"/>
     <mergeCell ref="A30:B31"/>
     <mergeCell ref="A32:B33"/>
@@ -934,15 +958,6 @@
     <mergeCell ref="A22:B23"/>
     <mergeCell ref="A24:B25"/>
     <mergeCell ref="A26:B27"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="A4:B5"/>
-    <mergeCell ref="A6:B7"/>
-    <mergeCell ref="A8:B9"/>
-    <mergeCell ref="A10:B11"/>
-    <mergeCell ref="A12:B13"/>
-    <mergeCell ref="A14:B15"/>
-    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>